<commit_message>
working on interventions, very slow
</commit_message>
<xml_diff>
--- a/rapid/country-data.xlsx
+++ b/rapid/country-data.xlsx
@@ -1628,12 +1628,12 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
+      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.65" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="19.86328125" customWidth="1"/>
+    <col min="1" max="1" width="27.265625" customWidth="1"/>
     <col min="2" max="2" width="9.06640625" customWidth="1"/>
     <col min="3" max="3" width="17.33203125" customWidth="1"/>
     <col min="4" max="4" width="15.19921875" customWidth="1"/>
@@ -5669,8 +5669,8 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:G179">
-    <sortCondition ref="A2:A179"/>
+  <sortState ref="A2:G175">
+    <sortCondition ref="A2:A175"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>